<commit_message>
Adding the new Test Maps to the dev branch and updating the gitignore
</commit_message>
<xml_diff>
--- a/AD-EYE/Experiments/Base_Map/Simulation/TArosparam.xlsx
+++ b/AD-EYE/Experiments/Base_Map/Simulation/TArosparam.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adeye\AD-EYE_Core\AD-EYE\Experiments\Base_Map\Simulation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{497E3EB8-2A18-4887-A563-0B83F7AA22EB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64877862-C39C-4D00-A04F-B39E7C7EAB71}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -495,12 +495,6 @@
     <t>remove_points_upto</t>
   </si>
   <si>
-    <t>$(env HOME)/AD-EYE_Core/AD-EYE/Data/ssdcaffe_models/VGGNet/VOC0712/SSD_512x512/deploy.prototxt</t>
-  </si>
-  <si>
-    <t>$(env HOME)/AD-EYE_Core/AD-EYE/Data/ssdcaffe_models/VGGNet/VOC0712/SSD_512x512/VGG_VOC0712_SSD_512x512_iter_120000.caffemodel</t>
-  </si>
-  <si>
     <t>camera_info</t>
   </si>
   <si>
@@ -751,6 +745,12 @@
   </si>
   <si>
     <t>adeyeGoalMarkerSize</t>
+  </si>
+  <si>
+    <t>$(env HOME)/AD-EYE_Core/AD-EYE/Data/ssdcaffe_models/AD-EYE_SSD_Model/SSD_512x512/deploy.prototxt</t>
+  </si>
+  <si>
+    <t>$(env HOME)/AD-EYE_Core/AD-EYE/Data/ssdcaffe_models/AD-EYE_SSD_Model/SSD_512x512/VGG_Dataset_SSD_512x512_iter_60000.caffemodel</t>
   </si>
 </sst>
 </file>
@@ -1147,8 +1147,8 @@
   </sheetPr>
   <dimension ref="A1:G237"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A166" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C189" sqref="C189"/>
+    <sheetView tabSelected="1" topLeftCell="A108" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G132" sqref="G132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1166,33 +1166,33 @@
         <v>6</v>
       </c>
       <c r="B1" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>203</v>
+      </c>
+      <c r="D1" s="10" t="s">
         <v>204</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="E1" s="10" t="s">
         <v>205</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>206</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="G1" s="10" t="s">
         <v>207</v>
-      </c>
-      <c r="F1" s="10" t="s">
-        <v>208</v>
-      </c>
-      <c r="G1" s="10" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B2" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>217</v>
-      </c>
-      <c r="B2" s="10" t="s">
-        <v>218</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>219</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>20</v>
@@ -1205,13 +1205,13 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B3" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>218</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>220</v>
       </c>
       <c r="D3" s="10" t="s">
         <v>19</v>
@@ -1219,7 +1219,7 @@
       <c r="E3" s="10"/>
       <c r="F3" s="10"/>
       <c r="G3" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1227,7 +1227,7 @@
         <v>22</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>0</v>
@@ -1250,7 +1250,7 @@
         <v>22</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>1</v>
@@ -1273,7 +1273,7 @@
         <v>22</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>2</v>
@@ -1296,10 +1296,10 @@
         <v>22</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D7" s="5" t="s">
         <v>5</v>
@@ -1319,7 +1319,7 @@
         <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>3</v>
@@ -1342,7 +1342,7 @@
         <v>22</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>4</v>
@@ -1365,10 +1365,10 @@
         <v>22</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D10" s="5" t="s">
         <v>19</v>
@@ -1376,7 +1376,7 @@
       <c r="E10" s="5"/>
       <c r="F10" s="5"/>
       <c r="G10" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1384,7 +1384,7 @@
         <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C11" s="4" t="s">
         <v>7</v>
@@ -1407,7 +1407,7 @@
         <v>22</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C12" s="4" t="s">
         <v>66</v>
@@ -1430,7 +1430,7 @@
         <v>22</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C13" s="4" t="s">
         <v>8</v>
@@ -1453,7 +1453,7 @@
         <v>22</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C14" s="4" t="s">
         <v>9</v>
@@ -1472,7 +1472,7 @@
         <v>22</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C15" s="4" t="s">
         <v>10</v>
@@ -1491,7 +1491,7 @@
         <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>11</v>
@@ -1510,7 +1510,7 @@
         <v>22</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>12</v>
@@ -1529,7 +1529,7 @@
         <v>22</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C18" s="4" t="s">
         <v>13</v>
@@ -1548,7 +1548,7 @@
         <v>22</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>14</v>
@@ -1571,7 +1571,7 @@
         <v>22</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C20" s="4" t="s">
         <v>15</v>
@@ -1590,7 +1590,7 @@
         <v>22</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>16</v>
@@ -1609,7 +1609,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>17</v>
@@ -1628,7 +1628,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>18</v>
@@ -1644,10 +1644,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>0</v>
@@ -1662,15 +1662,15 @@
         <v>10</v>
       </c>
       <c r="G24" s="11" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>1</v>
@@ -1690,10 +1690,10 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>2</v>
@@ -1708,18 +1708,18 @@
         <v>10</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="D27" s="5" t="s">
         <v>5</v>
@@ -1736,10 +1736,10 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C28" s="4" t="s">
         <v>3</v>
@@ -1759,10 +1759,10 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>4</v>
@@ -1782,13 +1782,13 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="D30" s="5" t="s">
         <v>19</v>
@@ -1796,15 +1796,15 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>7</v>
@@ -1819,15 +1819,15 @@
         <v>10</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C32" s="4" t="s">
         <v>66</v>
@@ -1850,7 +1850,7 @@
         <v>23</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C33" s="4" t="s">
         <v>0</v>
@@ -1873,7 +1873,7 @@
         <v>23</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C34" s="4" t="s">
         <v>1</v>
@@ -1896,7 +1896,7 @@
         <v>23</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C35" s="4" t="s">
         <v>2</v>
@@ -1919,7 +1919,7 @@
         <v>23</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C36" s="4" t="s">
         <v>69</v>
@@ -1942,7 +1942,7 @@
         <v>23</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C37" s="4" t="s">
         <v>70</v>
@@ -1965,7 +1965,7 @@
         <v>23</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C38" s="4" t="s">
         <v>71</v>
@@ -1988,7 +1988,7 @@
         <v>23</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C39" s="4" t="s">
         <v>72</v>
@@ -2011,7 +2011,7 @@
         <v>23</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C40" s="4" t="s">
         <v>0</v>
@@ -2034,7 +2034,7 @@
         <v>23</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C41" s="4" t="s">
         <v>1</v>
@@ -2057,7 +2057,7 @@
         <v>23</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C42" s="4" t="s">
         <v>2</v>
@@ -2080,7 +2080,7 @@
         <v>23</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C43" s="4" t="s">
         <v>69</v>
@@ -2103,7 +2103,7 @@
         <v>23</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C44" s="4" t="s">
         <v>70</v>
@@ -2126,7 +2126,7 @@
         <v>23</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C45" s="4" t="s">
         <v>71</v>
@@ -2149,7 +2149,7 @@
         <v>23</v>
       </c>
       <c r="B46" s="3" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C46" s="4" t="s">
         <v>72</v>
@@ -2172,10 +2172,10 @@
         <v>23</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D47" s="5" t="s">
         <v>19</v>
@@ -2183,7 +2183,7 @@
       <c r="E47" s="5"/>
       <c r="F47" s="5"/>
       <c r="G47" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
@@ -2191,10 +2191,10 @@
         <v>23</v>
       </c>
       <c r="B48" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="C48" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>160</v>
       </c>
       <c r="D48" s="5" t="s">
         <v>19</v>
@@ -2210,10 +2210,10 @@
         <v>23</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D49" s="5" t="s">
         <v>19</v>
@@ -2221,7 +2221,7 @@
       <c r="E49" s="5"/>
       <c r="F49" s="5"/>
       <c r="G49" s="4" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2229,10 +2229,10 @@
         <v>23</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D50" s="5" t="s">
         <v>20</v>
@@ -2250,7 +2250,7 @@
         <v>23</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C51" s="4" t="s">
         <v>50</v>
@@ -2271,10 +2271,10 @@
         <v>23</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D52" s="5" t="s">
         <v>5</v>
@@ -2292,10 +2292,10 @@
         <v>23</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C53" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D53" s="5" t="s">
         <v>5</v>
@@ -2313,10 +2313,10 @@
         <v>23</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>5</v>
@@ -2334,10 +2334,10 @@
         <v>23</v>
       </c>
       <c r="B55" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C55" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D55" s="5" t="s">
         <v>5</v>
@@ -2355,10 +2355,10 @@
         <v>23</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D56" s="5" t="s">
         <v>5</v>
@@ -2376,10 +2376,10 @@
         <v>23</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D57" s="5" t="s">
         <v>5</v>
@@ -2397,10 +2397,10 @@
         <v>23</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>5</v>
@@ -2418,10 +2418,10 @@
         <v>23</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C59" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>5</v>
@@ -2439,10 +2439,10 @@
         <v>23</v>
       </c>
       <c r="B60" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C60" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D60" s="5" t="s">
         <v>5</v>
@@ -2460,10 +2460,10 @@
         <v>23</v>
       </c>
       <c r="B61" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D61" s="5" t="s">
         <v>5</v>
@@ -2481,10 +2481,10 @@
         <v>23</v>
       </c>
       <c r="B62" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D62" s="5" t="s">
         <v>5</v>
@@ -2502,10 +2502,10 @@
         <v>23</v>
       </c>
       <c r="B63" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>5</v>
@@ -2523,10 +2523,10 @@
         <v>23</v>
       </c>
       <c r="B64" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D64" s="5" t="s">
         <v>5</v>
@@ -2544,10 +2544,10 @@
         <v>23</v>
       </c>
       <c r="B65" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D65" s="5" t="s">
         <v>5</v>
@@ -2565,10 +2565,10 @@
         <v>23</v>
       </c>
       <c r="B66" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C66" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D66" s="5" t="s">
         <v>5</v>
@@ -2586,10 +2586,10 @@
         <v>23</v>
       </c>
       <c r="B67" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C67" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>5</v>
@@ -2607,10 +2607,10 @@
         <v>23</v>
       </c>
       <c r="B68" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>5</v>
@@ -2628,10 +2628,10 @@
         <v>23</v>
       </c>
       <c r="B69" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C69" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D69" s="5" t="s">
         <v>5</v>
@@ -2649,10 +2649,10 @@
         <v>23</v>
       </c>
       <c r="B70" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D70" s="5" t="s">
         <v>5</v>
@@ -2670,10 +2670,10 @@
         <v>23</v>
       </c>
       <c r="B71" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C71" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D71" s="5" t="s">
         <v>5</v>
@@ -2691,10 +2691,10 @@
         <v>23</v>
       </c>
       <c r="B72" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C72" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>5</v>
@@ -2712,10 +2712,10 @@
         <v>23</v>
       </c>
       <c r="B73" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C73" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D73" s="5" t="s">
         <v>5</v>
@@ -2733,10 +2733,10 @@
         <v>23</v>
       </c>
       <c r="B74" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C74" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D74" s="5" t="s">
         <v>5</v>
@@ -2754,10 +2754,10 @@
         <v>23</v>
       </c>
       <c r="B75" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C75" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D75" s="5" t="s">
         <v>5</v>
@@ -2775,10 +2775,10 @@
         <v>23</v>
       </c>
       <c r="B76" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>5</v>
@@ -2796,10 +2796,10 @@
         <v>23</v>
       </c>
       <c r="B77" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D77" s="5" t="s">
         <v>5</v>
@@ -2817,10 +2817,10 @@
         <v>23</v>
       </c>
       <c r="B78" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C78" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D78" s="5" t="s">
         <v>5</v>
@@ -2838,10 +2838,10 @@
         <v>23</v>
       </c>
       <c r="B79" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D79" s="5" t="s">
         <v>5</v>
@@ -2859,10 +2859,10 @@
         <v>23</v>
       </c>
       <c r="B80" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C80" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D80" s="5" t="s">
         <v>5</v>
@@ -2880,10 +2880,10 @@
         <v>23</v>
       </c>
       <c r="B81" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C81" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D81" s="5" t="s">
         <v>5</v>
@@ -2901,10 +2901,10 @@
         <v>23</v>
       </c>
       <c r="B82" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D82" s="5" t="s">
         <v>5</v>
@@ -2922,10 +2922,10 @@
         <v>23</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C83" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D83" s="5" t="s">
         <v>5</v>
@@ -2943,10 +2943,10 @@
         <v>23</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D84" s="5" t="s">
         <v>5</v>
@@ -2964,10 +2964,10 @@
         <v>23</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D85" s="5" t="s">
         <v>5</v>
@@ -2985,10 +2985,10 @@
         <v>23</v>
       </c>
       <c r="B86" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C86" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D86" s="5" t="s">
         <v>5</v>
@@ -3006,10 +3006,10 @@
         <v>23</v>
       </c>
       <c r="B87" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D87" s="5" t="s">
         <v>19</v>
@@ -3017,7 +3017,7 @@
       <c r="E87" s="5"/>
       <c r="F87" s="5"/>
       <c r="G87" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
@@ -3025,10 +3025,10 @@
         <v>23</v>
       </c>
       <c r="B88" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D88" s="5" t="s">
         <v>19</v>
@@ -3036,7 +3036,7 @@
       <c r="E88" s="5"/>
       <c r="F88" s="5"/>
       <c r="G88" s="4" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
@@ -3044,10 +3044,10 @@
         <v>23</v>
       </c>
       <c r="B89" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D89" s="5" t="s">
         <v>19</v>
@@ -3055,7 +3055,7 @@
       <c r="E89" s="5"/>
       <c r="F89" s="5"/>
       <c r="G89" s="4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
@@ -3063,10 +3063,10 @@
         <v>23</v>
       </c>
       <c r="B90" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D90" s="5" t="s">
         <v>20</v>
@@ -3084,7 +3084,7 @@
         <v>23</v>
       </c>
       <c r="B91" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C91" s="4" t="s">
         <v>50</v>
@@ -3105,10 +3105,10 @@
         <v>23</v>
       </c>
       <c r="B92" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C92" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D92" s="5" t="s">
         <v>5</v>
@@ -3126,10 +3126,10 @@
         <v>23</v>
       </c>
       <c r="B93" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D93" s="5" t="s">
         <v>5</v>
@@ -3147,10 +3147,10 @@
         <v>23</v>
       </c>
       <c r="B94" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C94" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D94" s="5" t="s">
         <v>5</v>
@@ -3168,10 +3168,10 @@
         <v>23</v>
       </c>
       <c r="B95" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D95" s="5" t="s">
         <v>5</v>
@@ -3189,10 +3189,10 @@
         <v>23</v>
       </c>
       <c r="B96" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C96" s="4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D96" s="5" t="s">
         <v>5</v>
@@ -3210,10 +3210,10 @@
         <v>23</v>
       </c>
       <c r="B97" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C97" s="4" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D97" s="5" t="s">
         <v>5</v>
@@ -3231,10 +3231,10 @@
         <v>23</v>
       </c>
       <c r="B98" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C98" s="4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D98" s="5" t="s">
         <v>5</v>
@@ -3252,10 +3252,10 @@
         <v>23</v>
       </c>
       <c r="B99" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C99" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D99" s="5" t="s">
         <v>5</v>
@@ -3273,10 +3273,10 @@
         <v>23</v>
       </c>
       <c r="B100" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C100" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="D100" s="5" t="s">
         <v>5</v>
@@ -3294,10 +3294,10 @@
         <v>23</v>
       </c>
       <c r="B101" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C101" s="4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="D101" s="5" t="s">
         <v>5</v>
@@ -3315,10 +3315,10 @@
         <v>23</v>
       </c>
       <c r="B102" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C102" s="4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D102" s="5" t="s">
         <v>5</v>
@@ -3336,10 +3336,10 @@
         <v>23</v>
       </c>
       <c r="B103" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C103" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D103" s="5" t="s">
         <v>5</v>
@@ -3357,10 +3357,10 @@
         <v>23</v>
       </c>
       <c r="B104" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C104" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D104" s="5" t="s">
         <v>5</v>
@@ -3378,10 +3378,10 @@
         <v>23</v>
       </c>
       <c r="B105" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C105" s="4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D105" s="5" t="s">
         <v>5</v>
@@ -3399,10 +3399,10 @@
         <v>23</v>
       </c>
       <c r="B106" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C106" s="4" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="D106" s="5" t="s">
         <v>5</v>
@@ -3420,10 +3420,10 @@
         <v>23</v>
       </c>
       <c r="B107" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C107" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D107" s="5" t="s">
         <v>5</v>
@@ -3441,10 +3441,10 @@
         <v>23</v>
       </c>
       <c r="B108" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C108" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="D108" s="5" t="s">
         <v>5</v>
@@ -3462,10 +3462,10 @@
         <v>23</v>
       </c>
       <c r="B109" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C109" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="D109" s="5" t="s">
         <v>5</v>
@@ -3483,10 +3483,10 @@
         <v>23</v>
       </c>
       <c r="B110" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C110" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D110" s="5" t="s">
         <v>5</v>
@@ -3504,10 +3504,10 @@
         <v>23</v>
       </c>
       <c r="B111" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C111" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="D111" s="5" t="s">
         <v>5</v>
@@ -3525,10 +3525,10 @@
         <v>23</v>
       </c>
       <c r="B112" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C112" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D112" s="5" t="s">
         <v>5</v>
@@ -3546,10 +3546,10 @@
         <v>23</v>
       </c>
       <c r="B113" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C113" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="D113" s="5" t="s">
         <v>5</v>
@@ -3567,10 +3567,10 @@
         <v>23</v>
       </c>
       <c r="B114" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C114" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D114" s="5" t="s">
         <v>5</v>
@@ -3588,10 +3588,10 @@
         <v>23</v>
       </c>
       <c r="B115" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C115" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="D115" s="5" t="s">
         <v>5</v>
@@ -3609,10 +3609,10 @@
         <v>23</v>
       </c>
       <c r="B116" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C116" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D116" s="5" t="s">
         <v>5</v>
@@ -3630,10 +3630,10 @@
         <v>23</v>
       </c>
       <c r="B117" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C117" s="4" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="D117" s="5" t="s">
         <v>5</v>
@@ -3651,10 +3651,10 @@
         <v>23</v>
       </c>
       <c r="B118" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C118" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D118" s="5" t="s">
         <v>5</v>
@@ -3672,10 +3672,10 @@
         <v>23</v>
       </c>
       <c r="B119" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C119" s="4" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="D119" s="5" t="s">
         <v>5</v>
@@ -3693,10 +3693,10 @@
         <v>23</v>
       </c>
       <c r="B120" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C120" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D120" s="5" t="s">
         <v>5</v>
@@ -3714,10 +3714,10 @@
         <v>23</v>
       </c>
       <c r="B121" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C121" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="D121" s="5" t="s">
         <v>5</v>
@@ -3735,10 +3735,10 @@
         <v>23</v>
       </c>
       <c r="B122" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C122" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D122" s="5" t="s">
         <v>5</v>
@@ -3756,10 +3756,10 @@
         <v>23</v>
       </c>
       <c r="B123" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C123" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="D123" s="5" t="s">
         <v>5</v>
@@ -3777,10 +3777,10 @@
         <v>23</v>
       </c>
       <c r="B124" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C124" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D124" s="5" t="s">
         <v>5</v>
@@ -3798,10 +3798,10 @@
         <v>23</v>
       </c>
       <c r="B125" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C125" s="4" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D125" s="5" t="s">
         <v>5</v>
@@ -3819,10 +3819,10 @@
         <v>23</v>
       </c>
       <c r="B126" s="2" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="C126" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D126" s="5" t="s">
         <v>5</v>
@@ -3840,7 +3840,7 @@
         <v>23</v>
       </c>
       <c r="B127" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C127" s="4" t="s">
         <v>73</v>
@@ -3859,7 +3859,7 @@
         <v>23</v>
       </c>
       <c r="B128" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C128" s="4" t="s">
         <v>74</v>
@@ -3882,7 +3882,7 @@
         <v>23</v>
       </c>
       <c r="B129" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C129" s="4" t="s">
         <v>75</v>
@@ -3905,7 +3905,7 @@
         <v>23</v>
       </c>
       <c r="B130" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C130" s="4" t="s">
         <v>76</v>
@@ -3916,7 +3916,7 @@
       <c r="E130" s="5"/>
       <c r="F130" s="5"/>
       <c r="G130" s="8" t="s">
-        <v>156</v>
+        <v>240</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
@@ -3924,7 +3924,7 @@
         <v>23</v>
       </c>
       <c r="B131" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C131" s="4" t="s">
         <v>77</v>
@@ -3935,7 +3935,7 @@
       <c r="E131" s="5"/>
       <c r="F131" s="5"/>
       <c r="G131" s="8" t="s">
-        <v>157</v>
+        <v>241</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
@@ -3943,7 +3943,7 @@
         <v>23</v>
       </c>
       <c r="B132" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C132" s="4" t="s">
         <v>78</v>
@@ -3962,7 +3962,7 @@
         <v>23</v>
       </c>
       <c r="B133" s="2" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C133" s="4" t="s">
         <v>79</v>
@@ -4919,10 +4919,10 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C181" s="4" t="s">
         <v>24</v>
@@ -4942,10 +4942,10 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B182" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C182" s="4" t="s">
         <v>25</v>
@@ -4961,10 +4961,10 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B183" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C183" s="4" t="s">
         <v>26</v>
@@ -4980,10 +4980,10 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B184" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C184" s="4" t="s">
         <v>27</v>
@@ -4999,10 +4999,10 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C185" s="4" t="s">
         <v>28</v>
@@ -5018,10 +5018,10 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B186" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C186" s="4" t="s">
         <v>29</v>
@@ -5041,10 +5041,10 @@
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B187" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C187" s="4" t="s">
         <v>30</v>
@@ -5064,10 +5064,10 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B188" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C188" s="4" t="s">
         <v>31</v>
@@ -5083,13 +5083,13 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="2" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C189" s="4" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="D189" s="5" t="s">
         <v>5</v>
@@ -5106,7 +5106,7 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B190" s="2" t="s">
         <v>65</v>
@@ -5129,7 +5129,7 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B191" s="2" t="s">
         <v>65</v>
@@ -5152,7 +5152,7 @@
     </row>
     <row r="192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A192" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B192" s="2" t="s">
         <v>65</v>
@@ -5175,7 +5175,7 @@
     </row>
     <row r="193" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A193" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B193" s="2" t="s">
         <v>65</v>
@@ -5198,7 +5198,7 @@
     </row>
     <row r="194" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A194" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B194" s="2" t="s">
         <v>65</v>
@@ -5221,7 +5221,7 @@
     </row>
     <row r="195" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A195" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B195" s="2" t="s">
         <v>65</v>
@@ -5244,7 +5244,7 @@
     </row>
     <row r="196" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A196" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B196" s="2" t="s">
         <v>65</v>
@@ -5267,7 +5267,7 @@
     </row>
     <row r="197" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A197" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B197" s="2" t="s">
         <v>65</v>
@@ -5290,7 +5290,7 @@
     </row>
     <row r="198" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A198" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B198" s="2" t="s">
         <v>65</v>
@@ -5313,7 +5313,7 @@
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A199" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B199" s="2" t="s">
         <v>65</v>
@@ -5336,7 +5336,7 @@
     </row>
     <row r="200" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A200" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B200" s="2" t="s">
         <v>65</v>
@@ -5359,7 +5359,7 @@
     </row>
     <row r="201" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A201" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B201" s="2" t="s">
         <v>65</v>
@@ -5382,7 +5382,7 @@
     </row>
     <row r="202" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A202" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B202" s="2" t="s">
         <v>65</v>
@@ -5405,7 +5405,7 @@
     </row>
     <row r="203" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A203" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B203" s="2" t="s">
         <v>65</v>
@@ -5428,7 +5428,7 @@
     </row>
     <row r="204" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A204" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B204" s="2" t="s">
         <v>65</v>
@@ -5451,7 +5451,7 @@
     </row>
     <row r="205" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A205" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B205" s="2" t="s">
         <v>65</v>
@@ -5470,7 +5470,7 @@
     </row>
     <row r="206" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A206" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B206" s="2" t="s">
         <v>65</v>
@@ -5489,7 +5489,7 @@
     </row>
     <row r="207" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A207" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B207" s="2" t="s">
         <v>65</v>
@@ -5508,7 +5508,7 @@
     </row>
     <row r="208" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A208" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B208" s="2" t="s">
         <v>65</v>
@@ -5527,7 +5527,7 @@
     </row>
     <row r="209" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A209" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B209" s="2" t="s">
         <v>65</v>
@@ -5546,7 +5546,7 @@
     </row>
     <row r="210" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A210" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B210" s="2" t="s">
         <v>65</v>
@@ -5569,7 +5569,7 @@
     </row>
     <row r="211" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A211" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B211" s="2" t="s">
         <v>65</v>
@@ -5592,7 +5592,7 @@
     </row>
     <row r="212" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A212" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B212" s="2" t="s">
         <v>65</v>
@@ -5615,7 +5615,7 @@
     </row>
     <row r="213" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A213" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B213" s="2" t="s">
         <v>65</v>
@@ -5638,7 +5638,7 @@
     </row>
     <row r="214" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A214" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B214" s="2" t="s">
         <v>65</v>
@@ -5661,7 +5661,7 @@
     </row>
     <row r="215" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A215" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B215" s="2" t="s">
         <v>65</v>
@@ -5684,7 +5684,7 @@
     </row>
     <row r="216" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A216" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B216" s="2" t="s">
         <v>65</v>
@@ -5707,7 +5707,7 @@
     </row>
     <row r="217" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A217" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B217" s="2" t="s">
         <v>65</v>
@@ -5730,7 +5730,7 @@
     </row>
     <row r="218" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A218" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B218" s="2" t="s">
         <v>65</v>
@@ -5753,7 +5753,7 @@
     </row>
     <row r="219" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A219" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B219" s="2" t="s">
         <v>65</v>
@@ -5776,7 +5776,7 @@
     </row>
     <row r="220" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A220" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B220" s="2" t="s">
         <v>65</v>
@@ -5799,7 +5799,7 @@
     </row>
     <row r="221" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A221" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B221" s="2" t="s">
         <v>65</v>
@@ -5822,7 +5822,7 @@
     </row>
     <row r="222" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A222" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B222" s="2" t="s">
         <v>64</v>
@@ -5841,7 +5841,7 @@
     </row>
     <row r="223" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A223" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B223" s="2" t="s">
         <v>64</v>
@@ -5860,7 +5860,7 @@
     </row>
     <row r="224" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A224" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B224" s="2" t="s">
         <v>143</v>
@@ -5879,7 +5879,7 @@
     </row>
     <row r="225" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A225" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B225" s="2" t="s">
         <v>143</v>
@@ -5902,7 +5902,7 @@
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A226" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B226" s="2" t="s">
         <v>143</v>
@@ -5925,7 +5925,7 @@
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B227" s="4" t="s">
         <v>145</v>
@@ -5948,10 +5948,10 @@
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C228" s="4" t="s">
         <v>147</v>
@@ -5971,10 +5971,10 @@
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C229" s="4" t="s">
         <v>148</v>
@@ -5994,10 +5994,10 @@
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A230" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C230" s="4" t="s">
         <v>149</v>
@@ -6017,10 +6017,10 @@
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A231" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C231" s="4" t="s">
         <v>150</v>
@@ -6040,10 +6040,10 @@
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A232" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C232" s="4" t="s">
         <v>151</v>
@@ -6063,10 +6063,10 @@
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A233" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C233" s="4" t="s">
         <v>152</v>
@@ -6086,10 +6086,10 @@
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A234" s="2" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C234" s="4" t="s">
         <v>153</v>
@@ -6109,13 +6109,13 @@
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A235" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C235" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D235" s="7" t="s">
         <v>19</v>
@@ -6123,18 +6123,18 @@
       <c r="E235" s="7"/>
       <c r="F235" s="7"/>
       <c r="G235" s="12" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="B236" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="C236" s="4" t="s">
         <v>232</v>
-      </c>
-      <c r="B236" s="7" t="s">
-        <v>233</v>
-      </c>
-      <c r="C236" s="4" t="s">
-        <v>234</v>
       </c>
       <c r="D236" s="7" t="s">
         <v>19</v>
@@ -6142,24 +6142,24 @@
       <c r="E236" s="7"/>
       <c r="F236" s="7"/>
       <c r="G236" s="6" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="2" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B237" s="7" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C237" s="4" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="D237" s="7" t="s">
         <v>19</v>
       </c>
       <c r="G237" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
   </sheetData>

</xml_diff>